<commit_message>
Update list of messages to be broken out.
</commit_message>
<xml_diff>
--- a/Subgroups/ASX/Extension Definition Exercises/ASX Sample Report Messages.xlsx
+++ b/Subgroups/ASX/Extension Definition Exercises/ASX Sample Report Messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosang\Documents\6 - SISO\C2SIMDocs\ASX\C2SIMArtifacts\Subgroups\ASX\Extension Definition Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD4A47E-DE2E-4D78-A07F-030C58E613DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090DCBEA-2D94-4808-85D1-38B3AF3B9F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{315F412D-A997-402A-95E2-E68C4026AE2E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>C2SIM Object</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>May use either repositoryReference and reportReference or URL</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Link to actual file.</t>
   </si>
 </sst>
 </file>
@@ -675,8 +681,8 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H1"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,6 +880,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C39" s="8"/>
     </row>

</xml_diff>

<commit_message>
Report for SIW and updates to Reports
</commit_message>
<xml_diff>
--- a/Subgroups/ASX/Extension Definition Exercises/ASX Sample Report Messages.xlsx
+++ b/Subgroups/ASX/Extension Definition Exercises/ASX Sample Report Messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosang\Documents\6 - SISO\C2SIMDocs\ASX\C2SIMArtifacts\Subgroups\ASX\Extension Definition Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855BC739-F49E-44E8-A3E1-E6B87D0811CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF919C5-CFC5-4695-8DFC-21D370DAC01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9672" yWindow="3876" windowWidth="17280" windowHeight="8880" xr2:uid="{315F412D-A997-402A-95E2-E68C4026AE2E}"/>
+    <workbookView xWindow="3516" yWindow="4848" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="5" xr2:uid="{315F412D-A997-402A-95E2-E68C4026AE2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Report MessageBody Fields" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="143">
   <si>
     <t>C2SIM Object</t>
   </si>
@@ -449,6 +449,27 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t>May be based on location of sensor.</t>
+  </si>
+  <si>
+    <t>analystComment</t>
+  </si>
+  <si>
+    <t>SensorObservation</t>
+  </si>
+  <si>
+    <t>Unit with Sensor</t>
+  </si>
+  <si>
+    <t>Observed entity's location (optional)</t>
+  </si>
+  <si>
+    <t>Sensors's  location</t>
   </si>
 </sst>
 </file>
@@ -903,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550962A6-F1BC-47E8-810D-6806D0787E57}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
@@ -2157,18 +2178,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA568A3-46B1-4A74-80DC-08293821698C}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="25.109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="38" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
@@ -2292,300 +2315,300 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D29" s="1" t="s">
+      <c r="B32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="G32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="1" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="1" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="5" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="G35" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>12</v>
+      <c r="C38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="D40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+      <c r="D41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="7" t="s">
+      <c r="B43" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>31</v>
+      <c r="G43" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D44" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>26</v>
+      <c r="D45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D47" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D49" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D50" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G49" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D53" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
+      <c r="D55" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D56" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D57" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D58" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D59" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B61" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2638,22 +2661,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C66366-AD5E-4882-A227-B373EE81662B}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="25.109375" style="1" customWidth="1"/>
     <col min="5" max="6" width="19.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="38" style="1" customWidth="1"/>
+    <col min="8" max="8" width="82.44140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -2706,310 +2729,384 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>12</v>
+      <c r="E25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E26" s="1" t="s">
-        <v>21</v>
+      <c r="E26" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="H29" s="1" t="s">
-        <v>20</v>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>10</v>
+      <c r="A30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="7" t="s">
         <v>39</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E37" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E41" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+      <c r="F41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E43" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E50" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E51" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E52" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E53" s="1" t="s">
+    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>